<commit_message>
fixed threadspec auto sort thread
</commit_message>
<xml_diff>
--- a/fungalmicrofluidics/Experimental/Fig_sorter.xlsx
+++ b/fungalmicrofluidics/Experimental/Fig_sorter.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveconcordia-my.sharepoint.com/personal/k_samla_live_concordia_ca/Documents/CASB-PhD/Gitbubble/fungalmicrofluidics_basement/fungalmicrofluidics/Experimental/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KENZA Folder\PYTHON\fungalmicrofluidics\fungalmicrofluidics\Experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="114_{3494F199-24FB-864A-9EA3-24F2B4B836CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FF42AAD-BC37-634D-B300-52F19E550AFA}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="7740" windowWidth="21580" windowHeight="15540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="7740" windowWidth="21585" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Fig_autosort" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Fig_DropV_wElec" sheetId="2" r:id="rId3"/>
     <sheet name="Fig_DropV_woElec" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="33">
   <si>
     <t>VRMS</t>
   </si>
@@ -46,9 +45,6 @@
   </si>
   <si>
     <t>ErrorType</t>
-  </si>
-  <si>
-    <t>time</t>
   </si>
   <si>
     <t>Reso</t>
@@ -128,12 +124,21 @@
   <si>
     <t>neg</t>
   </si>
+  <si>
+    <t>350Vpp, 60nL/s</t>
+  </si>
+  <si>
+    <t>Fluo 5uM</t>
+  </si>
+  <si>
+    <t>H2O blue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +681,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,7 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1011,423 +1016,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="E4">
+        <f>SUM(A4:D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="S13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="S14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="J15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="S15" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="T15" t="s">
+        <v>5</v>
+      </c>
+      <c r="U15" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O1" t="b">
-        <v>0</v>
-      </c>
-      <c r="P1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" t="b">
-        <v>1</v>
-      </c>
-      <c r="X1" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF1" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>650</v>
-      </c>
-      <c r="B2">
-        <v>90</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>550</v>
-      </c>
-      <c r="K2">
-        <v>90</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>450</v>
-      </c>
-      <c r="T2">
-        <v>80</v>
-      </c>
-      <c r="U2">
-        <v>0.1</v>
-      </c>
-      <c r="AB2">
-        <v>350</v>
-      </c>
-      <c r="AC2">
-        <v>60</v>
-      </c>
-      <c r="AD2">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>650</v>
-      </c>
-      <c r="B3">
-        <v>90</v>
-      </c>
-      <c r="J3">
-        <v>550</v>
-      </c>
-      <c r="K3">
-        <v>90</v>
-      </c>
-      <c r="S3">
-        <v>450</v>
-      </c>
-      <c r="T3">
-        <v>80</v>
-      </c>
-      <c r="AB3">
-        <v>350</v>
-      </c>
-      <c r="AC3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>650</v>
-      </c>
-      <c r="B4">
-        <v>90</v>
-      </c>
-      <c r="J4">
-        <v>550</v>
-      </c>
-      <c r="K4">
-        <v>90</v>
-      </c>
-      <c r="S4">
-        <v>450</v>
-      </c>
-      <c r="T4">
-        <v>80</v>
-      </c>
-      <c r="AB4">
-        <v>350</v>
-      </c>
-      <c r="AC4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>650</v>
-      </c>
-      <c r="B5">
-        <v>90</v>
-      </c>
-      <c r="J5">
-        <v>550</v>
-      </c>
-      <c r="K5">
-        <v>90</v>
-      </c>
-      <c r="S5">
-        <v>450</v>
-      </c>
-      <c r="T5">
-        <v>80</v>
-      </c>
-      <c r="AB5">
-        <v>350</v>
-      </c>
-      <c r="AC5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>650</v>
-      </c>
-      <c r="B6">
-        <v>90</v>
-      </c>
-      <c r="J6">
-        <v>550</v>
-      </c>
-      <c r="K6">
-        <v>90</v>
-      </c>
-      <c r="S6">
-        <v>450</v>
-      </c>
-      <c r="T6">
-        <v>80</v>
-      </c>
-      <c r="AB6">
-        <v>350</v>
-      </c>
-      <c r="AC6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>650</v>
-      </c>
-      <c r="B7">
-        <v>90</v>
-      </c>
-      <c r="J7">
-        <v>550</v>
-      </c>
-      <c r="K7">
-        <v>90</v>
-      </c>
-      <c r="S7">
-        <v>450</v>
-      </c>
-      <c r="T7">
-        <v>80</v>
-      </c>
-      <c r="AB7">
-        <v>350</v>
-      </c>
-      <c r="AC7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>650</v>
-      </c>
-      <c r="B8">
-        <v>90</v>
-      </c>
-      <c r="J8">
-        <v>550</v>
-      </c>
-      <c r="K8">
-        <v>90</v>
-      </c>
-      <c r="S8">
-        <v>450</v>
-      </c>
-      <c r="T8">
-        <v>80</v>
-      </c>
-      <c r="AB8">
-        <v>350</v>
-      </c>
-      <c r="AC8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>650</v>
-      </c>
-      <c r="B9">
-        <v>90</v>
-      </c>
-      <c r="J9">
-        <v>550</v>
-      </c>
-      <c r="K9">
-        <v>90</v>
-      </c>
-      <c r="S9">
-        <v>450</v>
-      </c>
-      <c r="T9">
-        <v>80</v>
-      </c>
-      <c r="AB9">
-        <v>350</v>
-      </c>
-      <c r="AC9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" t="s">
-        <v>9</v>
-      </c>
-      <c r="S13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="J14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="9"/>
-      <c r="S14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="V14" s="9"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="V15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-      <c r="S15" t="s">
-        <v>5</v>
-      </c>
-      <c r="T15" t="s">
-        <v>6</v>
-      </c>
-      <c r="U15" t="s">
-        <v>5</v>
-      </c>
-      <c r="V15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E16">
-        <f>SUM(A16:D16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>60</v>
       </c>
@@ -1435,7 +1114,7 @@
         <v>0.133303</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>65</v>
       </c>
@@ -1443,7 +1122,7 @@
         <v>6.6650999999999905E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>70</v>
       </c>
@@ -1451,7 +1130,7 @@
         <v>0.166627999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>75</v>
       </c>
@@ -1459,7 +1138,7 @@
         <v>9.9976999999999899E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>80</v>
       </c>
@@ -1467,7 +1146,7 @@
         <v>9.9976999999999899E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>85</v>
       </c>
@@ -1475,7 +1154,7 @@
         <v>9.9976999999999996E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>90</v>
       </c>
@@ -1483,7 +1162,7 @@
         <v>9.9976999999999899E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>95</v>
       </c>
@@ -1491,7 +1170,7 @@
         <v>9.9977000000000094E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>100</v>
       </c>
@@ -1502,8 +1181,8 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="U14:V14"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="S14:T14"/>
@@ -1514,16 +1193,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>50</v>
       </c>
@@ -1560,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1577,7 +1256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>50</v>
       </c>
@@ -1594,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>50</v>
       </c>
@@ -1611,7 +1290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>50</v>
       </c>
@@ -1622,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>50</v>
       </c>
@@ -1639,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>50</v>
       </c>
@@ -1650,7 +1329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>50</v>
       </c>
@@ -1661,7 +1340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>50</v>
       </c>
@@ -1678,7 +1357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>50</v>
       </c>
@@ -1689,7 +1368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>50</v>
       </c>
@@ -1700,7 +1379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>50</v>
       </c>
@@ -1717,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>50</v>
       </c>
@@ -1728,7 +1407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>50</v>
       </c>
@@ -1739,7 +1418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>50</v>
       </c>
@@ -1756,7 +1435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>50</v>
       </c>
@@ -1773,7 +1452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>50</v>
       </c>
@@ -1790,7 +1469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>50</v>
       </c>
@@ -1807,7 +1486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>50</v>
       </c>
@@ -1824,7 +1503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>50</v>
       </c>
@@ -1841,7 +1520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>50</v>
       </c>
@@ -1858,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>50</v>
       </c>
@@ -1875,7 +1554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>50</v>
       </c>
@@ -1892,7 +1571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1909,7 +1588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>50</v>
       </c>
@@ -1926,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1943,7 +1622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>50</v>
       </c>
@@ -1960,7 +1639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>150</v>
       </c>
@@ -1977,7 +1656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>150</v>
       </c>
@@ -1994,7 +1673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>150</v>
       </c>
@@ -2011,7 +1690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>150</v>
       </c>
@@ -2028,7 +1707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>150</v>
       </c>
@@ -2045,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>150</v>
       </c>
@@ -2062,7 +1741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>150</v>
       </c>
@@ -2079,7 +1758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>150</v>
       </c>
@@ -2096,7 +1775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>150</v>
       </c>
@@ -2113,10 +1792,10 @@
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>150</v>
       </c>
@@ -2133,10 +1812,10 @@
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>150</v>
       </c>
@@ -2153,10 +1832,10 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>150</v>
       </c>
@@ -2173,7 +1852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>150</v>
       </c>
@@ -2190,7 +1869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>150</v>
       </c>
@@ -2207,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>150</v>
       </c>
@@ -2224,7 +1903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>150</v>
       </c>
@@ -2241,7 +1920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>150</v>
       </c>
@@ -2258,7 +1937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>150</v>
       </c>
@@ -2275,7 +1954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>150</v>
       </c>
@@ -2292,7 +1971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>150</v>
       </c>
@@ -2309,7 +1988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>150</v>
       </c>
@@ -2326,7 +2005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>150</v>
       </c>
@@ -2343,7 +2022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>150</v>
       </c>
@@ -2360,7 +2039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>150</v>
       </c>
@@ -2377,7 +2056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>150</v>
       </c>
@@ -2394,7 +2073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>150</v>
       </c>
@@ -2411,7 +2090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>150</v>
       </c>
@@ -2428,7 +2107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>250</v>
       </c>
@@ -2445,7 +2124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>250</v>
       </c>
@@ -2462,7 +2141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>250</v>
       </c>
@@ -2479,7 +2158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>250</v>
       </c>
@@ -2496,7 +2175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>250</v>
       </c>
@@ -2507,7 +2186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>250</v>
       </c>
@@ -2524,7 +2203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>250</v>
       </c>
@@ -2535,7 +2214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>250</v>
       </c>
@@ -2546,7 +2225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>250</v>
       </c>
@@ -2563,7 +2242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>250</v>
       </c>
@@ -2574,7 +2253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>250</v>
       </c>
@@ -2585,7 +2264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>250</v>
       </c>
@@ -2602,7 +2281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>250</v>
       </c>
@@ -2613,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>250</v>
       </c>
@@ -2624,7 +2303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>250</v>
       </c>
@@ -2641,7 +2320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>250</v>
       </c>
@@ -2658,7 +2337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>250</v>
       </c>
@@ -2675,7 +2354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>250</v>
       </c>
@@ -2692,7 +2371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>250</v>
       </c>
@@ -2709,7 +2388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>250</v>
       </c>
@@ -2726,7 +2405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>250</v>
       </c>
@@ -2743,7 +2422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>250</v>
       </c>
@@ -2760,7 +2439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>250</v>
       </c>
@@ -2777,7 +2456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>250</v>
       </c>
@@ -2794,7 +2473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>250</v>
       </c>
@@ -2811,7 +2490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>250</v>
       </c>
@@ -2828,7 +2507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>250</v>
       </c>
@@ -2845,7 +2524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>350</v>
       </c>
@@ -2862,7 +2541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>350</v>
       </c>
@@ -2879,7 +2558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>350</v>
       </c>
@@ -2896,7 +2575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>350</v>
       </c>
@@ -2913,7 +2592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>350</v>
       </c>
@@ -2924,7 +2603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>350</v>
       </c>
@@ -2941,7 +2620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>350</v>
       </c>
@@ -2952,7 +2631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>350</v>
       </c>
@@ -2963,7 +2642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>350</v>
       </c>
@@ -2980,7 +2659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>350</v>
       </c>
@@ -2991,7 +2670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>350</v>
       </c>
@@ -3002,7 +2681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>350</v>
       </c>
@@ -3019,7 +2698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>350</v>
       </c>
@@ -3030,7 +2709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>350</v>
       </c>
@@ -3041,7 +2720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>350</v>
       </c>
@@ -3058,7 +2737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>350</v>
       </c>
@@ -3075,7 +2754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>350</v>
       </c>
@@ -3092,7 +2771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>350</v>
       </c>
@@ -3109,7 +2788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>350</v>
       </c>
@@ -3126,7 +2805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>350</v>
       </c>
@@ -3143,7 +2822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>350</v>
       </c>
@@ -3160,7 +2839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>350</v>
       </c>
@@ -3177,7 +2856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>350</v>
       </c>
@@ -3194,7 +2873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>350</v>
       </c>
@@ -3211,7 +2890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>350</v>
       </c>
@@ -3228,7 +2907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>350</v>
       </c>
@@ -3245,7 +2924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>350</v>
       </c>
@@ -3262,7 +2941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>450</v>
       </c>
@@ -3279,7 +2958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>450</v>
       </c>
@@ -3296,7 +2975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>450</v>
       </c>
@@ -3313,7 +2992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>450</v>
       </c>
@@ -3330,7 +3009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>450</v>
       </c>
@@ -3341,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>450</v>
       </c>
@@ -3358,7 +3037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>450</v>
       </c>
@@ -3369,7 +3048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>450</v>
       </c>
@@ -3380,7 +3059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>450</v>
       </c>
@@ -3397,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>450</v>
       </c>
@@ -3408,7 +3087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>450</v>
       </c>
@@ -3419,7 +3098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>450</v>
       </c>
@@ -3436,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>450</v>
       </c>
@@ -3447,7 +3126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>450</v>
       </c>
@@ -3458,7 +3137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>450</v>
       </c>
@@ -3475,7 +3154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>450</v>
       </c>
@@ -3492,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>450</v>
       </c>
@@ -3509,7 +3188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>450</v>
       </c>
@@ -3526,7 +3205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>450</v>
       </c>
@@ -3543,7 +3222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>450</v>
       </c>
@@ -3560,7 +3239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>450</v>
       </c>
@@ -3577,7 +3256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>450</v>
       </c>
@@ -3594,7 +3273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>450</v>
       </c>
@@ -3611,7 +3290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>450</v>
       </c>
@@ -3628,7 +3307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>450</v>
       </c>
@@ -3645,7 +3324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>450</v>
       </c>
@@ -3662,7 +3341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>450</v>
       </c>
@@ -3679,7 +3358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>550</v>
       </c>
@@ -3696,7 +3375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>550</v>
       </c>
@@ -3713,7 +3392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>550</v>
       </c>
@@ -3730,7 +3409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>550</v>
       </c>
@@ -3747,7 +3426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>550</v>
       </c>
@@ -3758,7 +3437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>550</v>
       </c>
@@ -3775,7 +3454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>550</v>
       </c>
@@ -3786,7 +3465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>550</v>
       </c>
@@ -3797,7 +3476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145">
         <v>550</v>
       </c>
@@ -3814,10 +3493,10 @@
         <v>10</v>
       </c>
       <c r="F145" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146">
         <v>550</v>
       </c>
@@ -3828,7 +3507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6">
       <c r="A147">
         <v>550</v>
       </c>
@@ -3839,7 +3518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148">
         <v>550</v>
       </c>
@@ -3856,10 +3535,10 @@
         <v>10</v>
       </c>
       <c r="F148" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149">
         <v>550</v>
       </c>
@@ -3870,7 +3549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150">
         <v>550</v>
       </c>
@@ -3881,7 +3560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151">
         <v>550</v>
       </c>
@@ -3898,10 +3577,10 @@
         <v>10</v>
       </c>
       <c r="F151" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152">
         <v>550</v>
       </c>
@@ -3918,7 +3597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153">
         <v>550</v>
       </c>
@@ -3935,7 +3614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6">
       <c r="A154">
         <v>550</v>
       </c>
@@ -3952,7 +3631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6">
       <c r="A155">
         <v>550</v>
       </c>
@@ -3969,7 +3648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6">
       <c r="A156">
         <v>550</v>
       </c>
@@ -3986,7 +3665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6">
       <c r="A157">
         <v>550</v>
       </c>
@@ -4003,7 +3682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6">
       <c r="A158">
         <v>550</v>
       </c>
@@ -4020,7 +3699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6">
       <c r="A159">
         <v>550</v>
       </c>
@@ -4037,7 +3716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6">
       <c r="A160">
         <v>550</v>
       </c>
@@ -4054,7 +3733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6">
       <c r="A161">
         <v>550</v>
       </c>
@@ -4071,7 +3750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6">
       <c r="A162">
         <v>550</v>
       </c>
@@ -4088,7 +3767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6">
       <c r="A163">
         <v>550</v>
       </c>
@@ -4105,7 +3784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6">
       <c r="A164">
         <v>650</v>
       </c>
@@ -4122,7 +3801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6">
       <c r="A165">
         <v>650</v>
       </c>
@@ -4139,7 +3818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6">
       <c r="A166">
         <v>650</v>
       </c>
@@ -4156,7 +3835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6">
       <c r="A167">
         <v>650</v>
       </c>
@@ -4173,7 +3852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6">
       <c r="A168">
         <v>650</v>
       </c>
@@ -4184,7 +3863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6">
       <c r="A169">
         <v>650</v>
       </c>
@@ -4201,7 +3880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6">
       <c r="A170">
         <v>650</v>
       </c>
@@ -4212,7 +3891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6">
       <c r="A171">
         <v>650</v>
       </c>
@@ -4223,7 +3902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6">
       <c r="A172">
         <v>650</v>
       </c>
@@ -4240,10 +3919,10 @@
         <v>10</v>
       </c>
       <c r="F172" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173">
         <v>650</v>
       </c>
@@ -4254,7 +3933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6">
       <c r="A174">
         <v>650</v>
       </c>
@@ -4265,7 +3944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6">
       <c r="A175">
         <v>650</v>
       </c>
@@ -4282,10 +3961,10 @@
         <v>10</v>
       </c>
       <c r="F175" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176">
         <v>650</v>
       </c>
@@ -4296,7 +3975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6">
       <c r="A177">
         <v>650</v>
       </c>
@@ -4307,7 +3986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6">
       <c r="A178">
         <v>650</v>
       </c>
@@ -4324,10 +4003,10 @@
         <v>10</v>
       </c>
       <c r="F178" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179">
         <v>650</v>
       </c>
@@ -4344,7 +4023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6">
       <c r="A180">
         <v>650</v>
       </c>
@@ -4361,7 +4040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6">
       <c r="A181">
         <v>650</v>
       </c>
@@ -4378,7 +4057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6">
       <c r="A182">
         <v>650</v>
       </c>
@@ -4395,7 +4074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6">
       <c r="A183">
         <v>650</v>
       </c>
@@ -4412,7 +4091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6">
       <c r="A184">
         <v>650</v>
       </c>
@@ -4429,7 +4108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6">
       <c r="A185">
         <v>650</v>
       </c>
@@ -4446,7 +4125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6">
       <c r="A186">
         <v>650</v>
       </c>
@@ -4463,7 +4142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6">
       <c r="A187">
         <v>650</v>
       </c>
@@ -4480,7 +4159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6">
       <c r="A188">
         <v>650</v>
       </c>
@@ -4497,7 +4176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6">
       <c r="A189">
         <v>650</v>
       </c>
@@ -4514,7 +4193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6">
       <c r="A190">
         <v>650</v>
       </c>
@@ -4537,109 +4216,109 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView topLeftCell="K4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="15.75">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:32" ht="15.75">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4">
         <v>650</v>
@@ -4705,7 +4384,7 @@
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
     </row>
-    <row r="3" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="15.75">
       <c r="A3" s="5"/>
       <c r="B3" s="4">
         <v>650</v>
@@ -4771,7 +4450,7 @@
       <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
     </row>
-    <row r="4" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="15.75">
       <c r="A4" s="5"/>
       <c r="B4" s="4">
         <v>650</v>
@@ -4837,7 +4516,7 @@
       <c r="AE4" s="5"/>
       <c r="AF4" s="5"/>
     </row>
-    <row r="5" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="15.75">
       <c r="A5" s="5"/>
       <c r="B5" s="4">
         <v>650</v>
@@ -4903,7 +4582,7 @@
       <c r="AE5" s="5"/>
       <c r="AF5" s="5"/>
     </row>
-    <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="15.75">
       <c r="A6" s="5"/>
       <c r="B6" s="4">
         <v>650</v>
@@ -4969,7 +4648,7 @@
       <c r="AE6" s="5"/>
       <c r="AF6" s="5"/>
     </row>
-    <row r="7" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" ht="15.75">
       <c r="A7" s="5"/>
       <c r="B7" s="4">
         <v>650</v>
@@ -5035,7 +4714,7 @@
       <c r="AE7" s="5"/>
       <c r="AF7" s="5"/>
     </row>
-    <row r="8" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" ht="15.75">
       <c r="A8" s="5"/>
       <c r="B8" s="4">
         <v>650</v>
@@ -5101,7 +4780,7 @@
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
     </row>
-    <row r="9" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" ht="15.75">
       <c r="A9" s="5"/>
       <c r="B9" s="4">
         <v>650</v>
@@ -5167,7 +4846,7 @@
       <c r="AE9" s="5"/>
       <c r="AF9" s="5"/>
     </row>
-    <row r="10" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="15.75">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -5201,7 +4880,7 @@
       <c r="AE10" s="5"/>
       <c r="AF10" s="5"/>
     </row>
-    <row r="11" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" ht="15.75">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -5214,16 +4893,16 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -5243,7 +4922,7 @@
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
     </row>
-    <row r="12" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" ht="15.75">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -5266,26 +4945,26 @@
         <v>1333.00783</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W12" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="X12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y12" s="5"/>
       <c r="Z12" s="5"/>
@@ -5296,7 +4975,7 @@
       <c r="AE12" s="5"/>
       <c r="AF12" s="5"/>
     </row>
-    <row r="13" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" ht="15.75">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -5319,7 +4998,7 @@
         <v>1574.1644799999999</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
@@ -5336,7 +5015,7 @@
         <v>904.54819000000009</v>
       </c>
       <c r="W13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X13" s="6"/>
       <c r="Y13" s="5"/>
@@ -5348,7 +5027,7 @@
       <c r="AE13" s="5"/>
       <c r="AF13" s="5"/>
     </row>
-    <row r="14" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="15.75">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -5370,7 +5049,7 @@
         <v>1735.5685899999999</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -5387,7 +5066,7 @@
         <v>943.87635999999998</v>
       </c>
       <c r="W14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X14" s="6"/>
       <c r="Y14" s="5"/>
@@ -5399,7 +5078,7 @@
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
     </row>
-    <row r="15" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="15.75">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -5421,7 +5100,7 @@
         <v>1458.3333099999998</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -5438,7 +5117,7 @@
         <v>1179.8454500000003</v>
       </c>
       <c r="W15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
@@ -5450,7 +5129,7 @@
       <c r="AE15" s="5"/>
       <c r="AF15" s="5"/>
     </row>
-    <row r="16" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="15.75">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -5472,7 +5151,7 @@
         <v>1984.3207299999999</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -5489,7 +5168,7 @@
         <v>1219.1736199999998</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X16" s="6"/>
       <c r="Y16" s="5"/>
@@ -5501,7 +5180,7 @@
       <c r="AE16" s="5"/>
       <c r="AF16" s="5"/>
     </row>
-    <row r="17" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="15.75">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -5523,7 +5202,7 @@
         <v>1230.46875</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -5540,7 +5219,7 @@
         <v>1179.8454500000003</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X17" s="6"/>
       <c r="Y17" s="5"/>
@@ -5552,7 +5231,7 @@
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
     </row>
-    <row r="18" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="15.75">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -5574,7 +5253,7 @@
         <v>1917.8602100000001</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
@@ -5591,7 +5270,7 @@
         <v>1140.51721</v>
       </c>
       <c r="W18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
@@ -5603,7 +5282,7 @@
       <c r="AE18" s="5"/>
       <c r="AF18" s="5"/>
     </row>
-    <row r="19" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" ht="15.75">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -5625,7 +5304,7 @@
         <v>1623.5351300000002</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
@@ -5642,7 +5321,7 @@
         <v>1116.17121</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X19" s="6"/>
       <c r="Y19" s="5"/>
@@ -5654,7 +5333,7 @@
       <c r="AE19" s="5"/>
       <c r="AF19" s="5"/>
     </row>
-    <row r="20" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" ht="15.75">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -5676,7 +5355,7 @@
         <v>1652.0182</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
@@ -5693,7 +5372,7 @@
         <v>1116.17121</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X20" s="6"/>
       <c r="Y20" s="5"/>
@@ -5705,7 +5384,7 @@
       <c r="AE20" s="5"/>
       <c r="AF20" s="5"/>
     </row>
-    <row r="21" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" ht="15.75">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -5727,7 +5406,7 @@
         <v>1325.4123399999999</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
@@ -5744,7 +5423,7 @@
         <v>1140.51721</v>
       </c>
       <c r="W21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X21" s="6"/>
       <c r="Y21" s="5"/>
@@ -5756,7 +5435,7 @@
       <c r="AE21" s="5"/>
       <c r="AF21" s="5"/>
     </row>
-    <row r="22" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="15.75">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -5778,7 +5457,7 @@
         <v>1219.07555</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
@@ -5795,7 +5474,7 @@
         <v>2048.8109599999998</v>
       </c>
       <c r="W22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X22" s="6"/>
       <c r="Y22" s="5"/>
@@ -5807,7 +5486,7 @@
       <c r="AE22" s="5"/>
       <c r="AF22" s="5"/>
     </row>
-    <row r="23" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="15.75">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -5829,7 +5508,7 @@
         <v>1283.6371799999999</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
@@ -5844,7 +5523,7 @@
         <v>1846.5517000000002</v>
       </c>
       <c r="W23" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X23" s="6"/>
       <c r="Y23" s="5"/>
@@ -5856,7 +5535,7 @@
       <c r="AE23" s="5"/>
       <c r="AF23" s="5"/>
     </row>
-    <row r="24" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="15.75">
       <c r="L24" s="5">
         <v>13</v>
       </c>
@@ -5868,7 +5547,7 @@
         <v>1338.70443</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T24" s="5">
         <v>12</v>
@@ -5881,10 +5560,10 @@
         <v>1271.6111799999999</v>
       </c>
       <c r="W24" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="15.75">
       <c r="L25">
         <v>14</v>
       </c>
@@ -5896,7 +5575,7 @@
         <v>1160.2105200000001</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T25" s="5">
         <v>13</v>
@@ -5909,10 +5588,10 @@
         <v>1382.1046399999998</v>
       </c>
       <c r="W25" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="15.75">
       <c r="L26">
         <v>15</v>
       </c>
@@ -5924,7 +5603,7 @@
         <v>1167.80601</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T26" s="5">
         <v>1</v>
@@ -5937,10 +5616,10 @@
         <v>889.56601999999987</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="15.75">
       <c r="L27">
         <v>16</v>
       </c>
@@ -5952,7 +5631,7 @@
         <v>1013.99739</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T27" s="5">
         <v>2</v>
@@ -5965,10 +5644,10 @@
         <v>820.27350999999999</v>
       </c>
       <c r="W27" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="15.75">
       <c r="L28">
         <v>17</v>
       </c>
@@ -5980,7 +5659,7 @@
         <v>831.70570000000009</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T28" s="5">
         <v>3</v>
@@ -5993,10 +5672,10 @@
         <v>764.09038999999984</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" ht="15.75">
       <c r="L29">
         <v>18</v>
       </c>
@@ -6008,7 +5687,7 @@
         <v>903.86281999999994</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T29" s="5">
         <v>4</v>
@@ -6021,10 +5700,10 @@
         <v>715.39832000000001</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" ht="15.75">
       <c r="L30" s="8">
         <v>1</v>
       </c>
@@ -6036,7 +5715,7 @@
         <v>1055.7725500000001</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T30" s="5">
         <v>5</v>
@@ -6049,10 +5728,10 @@
         <v>749.10821999999996</v>
       </c>
       <c r="W30" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" ht="15.75">
       <c r="L31">
         <v>2</v>
       </c>
@@ -6064,7 +5743,7 @@
         <v>1038.6827499999999</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T31" s="5">
         <v>6</v>
@@ -6077,10 +5756,10 @@
         <v>777.19977999999992</v>
       </c>
       <c r="W31" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="15.75">
       <c r="L32">
         <v>3</v>
       </c>
@@ -6092,7 +5771,7 @@
         <v>1118.4353599999999</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T32" s="5">
         <v>7</v>
@@ -6105,10 +5784,10 @@
         <v>726.63492999999994</v>
       </c>
       <c r="W32" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="12:23" ht="15.75">
       <c r="L33">
         <v>4</v>
       </c>
@@ -6120,7 +5799,7 @@
         <v>1164.0082299999999</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T33" s="5">
         <v>8</v>
@@ -6133,10 +5812,10 @@
         <v>773.45421999999996</v>
       </c>
       <c r="W33" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="12:23" ht="15.75">
       <c r="L34">
         <v>5</v>
       </c>
@@ -6148,7 +5827,7 @@
         <v>1074.7613100000001</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T34" s="5">
         <v>9</v>
@@ -6161,10 +5840,10 @@
         <v>728.50771000000009</v>
       </c>
       <c r="W34" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="12:23" ht="15.75">
       <c r="L35">
         <v>6</v>
       </c>
@@ -6176,7 +5855,7 @@
         <v>943.73915999999997</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T35" s="5">
         <v>10</v>
@@ -6189,10 +5868,10 @@
         <v>1016.91436</v>
       </c>
       <c r="W35" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="12:23" ht="15.75">
       <c r="L36">
         <v>7</v>
       </c>
@@ -6204,7 +5883,7 @@
         <v>698.78472999999997</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T36" s="5">
         <v>11</v>
@@ -6217,10 +5896,10 @@
         <v>958.85852999999986</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="12:23" ht="15.75">
       <c r="L37">
         <v>8</v>
       </c>
@@ -6232,7 +5911,7 @@
         <v>901.96400000000006</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T37" s="5">
         <v>12</v>
@@ -6245,10 +5924,10 @@
         <v>986.95008999999993</v>
       </c>
       <c r="W37" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="12:23" ht="15.75">
       <c r="L38">
         <v>9</v>
       </c>
@@ -6260,7 +5939,7 @@
         <v>936.14366999999993</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T38" s="5">
         <v>1</v>
@@ -6273,10 +5952,10 @@
         <v>719.67230999999992</v>
       </c>
       <c r="W38" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="12:23" ht="15.75">
       <c r="L39">
         <v>10</v>
       </c>
@@ -6288,7 +5967,7 @@
         <v>900.06511</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T39" s="5">
         <v>2</v>
@@ -6301,10 +5980,10 @@
         <v>704.48133000000007</v>
       </c>
       <c r="W39" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="12:23" ht="15.75">
       <c r="L40">
         <v>11</v>
       </c>
@@ -6316,7 +5995,7 @@
         <v>989.3121000000001</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T40" s="5">
         <v>3</v>
@@ -6329,10 +6008,10 @@
         <v>683.59375</v>
       </c>
       <c r="W40" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="12:23" ht="15.75">
       <c r="L41">
         <v>12</v>
       </c>
@@ -6344,7 +6023,7 @@
         <v>776.63844999999992</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T41" s="5">
         <v>4</v>
@@ -6357,10 +6036,10 @@
         <v>588.65016000000003</v>
       </c>
       <c r="W41" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="12:23" ht="15.75">
       <c r="L42">
         <v>13</v>
       </c>
@@ -6372,7 +6051,7 @@
         <v>525.98741999999993</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T42" s="5">
         <v>5</v>
@@ -6385,10 +6064,10 @@
         <v>508.89754999999997</v>
       </c>
       <c r="W42" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="12:23" ht="15.75">
       <c r="L43">
         <v>14</v>
       </c>
@@ -6400,7 +6079,7 @@
         <v>750.05426999999997</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T43" s="5">
         <v>6</v>
@@ -6413,10 +6092,10 @@
         <v>565.86368999999991</v>
       </c>
       <c r="W43" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="12:23" ht="15.75">
       <c r="L44">
         <v>15</v>
       </c>
@@ -6428,7 +6107,7 @@
         <v>685.49264000000005</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T44" s="5">
         <v>7</v>
@@ -6441,10 +6120,10 @@
         <v>1069.0646400000001</v>
       </c>
       <c r="W44" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="12:23" ht="15.75">
       <c r="L45">
         <v>16</v>
       </c>
@@ -6456,7 +6135,7 @@
         <v>748.15538000000004</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T45" s="5">
         <v>1</v>
@@ -6469,10 +6148,10 @@
         <v>1074.7613100000001</v>
       </c>
       <c r="W45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="12:23" ht="15.75">
       <c r="L46">
         <v>17</v>
       </c>
@@ -6484,7 +6163,7 @@
         <v>827.90799000000004</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T46" s="5">
         <v>2</v>
@@ -6497,10 +6176,10 @@
         <v>1146.9184299999999</v>
       </c>
       <c r="W46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="12:23" ht="15.75">
       <c r="L47">
         <v>18</v>
       </c>
@@ -6512,7 +6191,7 @@
         <v>660.80727999999988</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T47" s="5">
         <v>3</v>
@@ -6525,10 +6204,10 @@
         <v>1146.9184299999999</v>
       </c>
       <c r="W47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="12:23" ht="15.75">
       <c r="L48">
         <v>19</v>
       </c>
@@ -6540,7 +6219,7 @@
         <v>696.88584000000003</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T48" s="5">
         <v>4</v>
@@ -6553,10 +6232,10 @@
         <v>1127.9296700000002</v>
       </c>
       <c r="W48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="12:23" ht="15.75">
       <c r="L49">
         <v>20</v>
       </c>
@@ -6568,7 +6247,7 @@
         <v>489.90886000000006</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T49" s="5">
         <v>5</v>
@@ -6581,10 +6260,10 @@
         <v>1198.1879000000001</v>
       </c>
       <c r="W49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="12:23" ht="15.75">
       <c r="L50">
         <v>21</v>
       </c>
@@ -6596,7 +6275,7 @@
         <v>581.05466999999999</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T50" s="5">
         <v>6</v>
@@ -6609,10 +6288,10 @@
         <v>1760.2538800000002</v>
       </c>
       <c r="W50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="12:23" ht="15.75">
       <c r="L51">
         <v>22</v>
       </c>
@@ -6624,7 +6303,7 @@
         <v>619.03211999999996</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T51" s="5">
         <v>7</v>
@@ -6637,10 +6316,10 @@
         <v>1796.3324399999999</v>
       </c>
       <c r="W51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="12:23" ht="15.75">
       <c r="L52">
         <v>23</v>
       </c>
@@ -6652,7 +6331,7 @@
         <v>683.59375</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T52" s="5">
         <v>8</v>
@@ -6665,10 +6344,10 @@
         <v>1591.2543500000002</v>
       </c>
       <c r="W52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="12:23" ht="15.75">
       <c r="L53">
         <v>24</v>
       </c>
@@ -6680,10 +6359,10 @@
         <v>732.96440000000007</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="12:23" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="12:23" ht="15.75">
       <c r="L54">
         <v>25</v>
       </c>
@@ -6695,7 +6374,7 @@
         <v>780.43623000000002</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -6705,38 +6384,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="6"/>
       <c r="B2" s="6">
         <v>80</v>
@@ -6758,7 +6437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="6"/>
       <c r="B3" s="6">
         <v>80</v>
@@ -6780,7 +6459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="6"/>
       <c r="B4" s="6">
         <v>80</v>
@@ -6802,7 +6481,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="6"/>
       <c r="B5" s="6">
         <v>80</v>
@@ -6824,7 +6503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="6"/>
       <c r="B6" s="6">
         <v>80</v>
@@ -6846,7 +6525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="6"/>
       <c r="B7" s="6">
         <v>80</v>
@@ -6868,7 +6547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="6"/>
       <c r="B8" s="6">
         <v>80</v>
@@ -6890,7 +6569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="6"/>
       <c r="B9" s="6">
         <v>80</v>
@@ -6918,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="C10" s="7">
         <v>2</v>
       </c>
@@ -6938,24 +6617,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="15.75">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="J11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11">
         <f>SUM(M9:M10)</f>
@@ -6965,7 +6644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="D12" s="7">
         <v>345</v>
       </c>
@@ -6973,37 +6652,37 @@
         <v>2</v>
       </c>
       <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
         <v>29</v>
       </c>
-      <c r="N12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14">
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M13">
         <f>3/277</f>
         <v>1.0830324909747292E-2</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="9">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="D14">
         <f>2/345</f>
         <v>5.7971014492753624E-3</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:12">
       <c r="J17">
         <f>5/(345+277)</f>
         <v>8.0385852090032149E-3</v>

</xml_diff>